<commit_message>
adding random slopes to create_formula and create_ulam_formula functions
</commit_message>
<xml_diff>
--- a/inst/example model control.xlsx
+++ b/inst/example model control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\mostlytidyMMM\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF959A-C16F-45D3-A14C-5384E6017F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2846C569-8B83-4764-A2FB-8D7BA4106953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
   <sheets>
     <sheet name="workflow" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>start_name</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>random slopes</t>
+  </si>
+  <si>
+    <t>list_rand_slopes</t>
+  </si>
+  <si>
+    <t>(1|store)</t>
+  </si>
+  <si>
+    <t>(TV1|store), (TV2|store)</t>
   </si>
 </sst>
 </file>
@@ -559,19 +571,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="108.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.31640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="108.3515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -582,7 +595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -593,29 +606,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -626,7 +639,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
@@ -635,6 +648,17 @@
       </c>
       <c r="C6" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -646,18 +670,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F036211F-86F5-4F9C-85F9-C4D9573482AB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="35.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.76953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.52734375" customWidth="1"/>
+    <col min="4" max="4" width="10.76171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -703,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -717,7 +741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -731,7 +755,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -742,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -765,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -788,7 +812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -811,7 +835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -834,7 +858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -848,7 +872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -862,7 +886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -876,7 +900,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -904,17 +928,17 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.2265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.52734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.52734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -937,7 +961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -960,7 +984,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -996,9 +1020,9 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
finishing the hyperparameter and formula tuning vignette
</commit_message>
<xml_diff>
--- a/inst/example model control.xlsx
+++ b/inst/example model control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\mostlytidyMMM\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2846C569-8B83-4764-A2FB-8D7BA4106953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A43EBC-0735-43AD-9ACF-982C16B0292F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>start_name</t>
   </si>
@@ -178,12 +178,6 @@
     <t>Which variable are we modeling?</t>
   </si>
   <si>
-    <t>add_trend</t>
-  </si>
-  <si>
-    <t>Estimate a trend effect using the trend (role 2 = 'trend) variable?</t>
-  </si>
-  <si>
     <t>trend</t>
   </si>
   <si>
@@ -202,7 +196,31 @@
     <t>(1|store)</t>
   </si>
   <si>
-    <t>(TV1|store), (TV2|store)</t>
+    <t>saved hyper parameter tibble</t>
+  </si>
+  <si>
+    <t>saved_hypers_filename</t>
+  </si>
+  <si>
+    <t>Find best seasonality spec?</t>
+  </si>
+  <si>
+    <t>search_seasonality</t>
+  </si>
+  <si>
+    <t>seasonality interactions to test?</t>
+  </si>
+  <si>
+    <t>interaction_fft</t>
+  </si>
+  <si>
+    <t>search_randoms</t>
+  </si>
+  <si>
+    <t>(TV1|store)</t>
+  </si>
+  <si>
+    <t>should different random effects be tested?</t>
   </si>
 </sst>
 </file>
@@ -226,18 +244,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -252,11 +264,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -597,68 +608,98 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+        <v>56</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -749,10 +790,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.5">
@@ -902,16 +943,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1024,16 +1065,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>